<commit_message>
Changes made to ScheduleApproximation.xlsx file
</commit_message>
<xml_diff>
--- a/ScheduleApproximation.xlsx
+++ b/ScheduleApproximation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s538339\Documents\GDP-1\health-wellness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E03E9EC-B1CF-4ED8-9E69-55698E8E463D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F424F49-70D2-4E4F-A8B5-089B23888D3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83925983-7E47-4241-A59F-1E401A86CA2F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <r>
       <t xml:space="preserve">                                                                                                                                                 </t>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t xml:space="preserve">           8/23/2020</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Working Hours</t>
   </si>
 </sst>
 </file>
@@ -203,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -249,6 +255,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,27 +577,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629B0EE5-2389-44FF-B5B1-1268CBE07ED8}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="44.90625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" customWidth="1"/>
-    <col min="11" max="11" width="18.36328125" customWidth="1"/>
+    <col min="3" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" customWidth="1"/>
+    <col min="12" max="12" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,8 +611,9 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -609,41 +624,44 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -653,32 +671,33 @@
       <c r="C5" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="31"/>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5">
-        <v>1.5</v>
-      </c>
       <c r="F5">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>1.5</v>
       </c>
       <c r="K5">
+        <v>1.5</v>
+      </c>
+      <c r="L5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -688,32 +707,33 @@
       <c r="C6" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
       <c r="F6">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H6">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="I6">
         <v>1.5</v>
       </c>
       <c r="J6">
+        <v>1.5</v>
+      </c>
+      <c r="K6">
         <v>1</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>9.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -723,14 +743,12 @@
       <c r="C7" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="32"/>
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
       <c r="F7">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>1.5</v>
@@ -739,16 +757,19 @@
         <v>1.5</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J7">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K7">
+        <v>1.5</v>
+      </c>
+      <c r="L7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -758,17 +779,18 @@
       <c r="C8" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="31"/>
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>7</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -778,32 +800,33 @@
       <c r="C9" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="31"/>
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="E9">
-        <v>1.5</v>
-      </c>
       <c r="F9">
         <v>1.5</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
       <c r="I9">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
         <v>10.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -813,17 +836,18 @@
       <c r="C10" s="25">
         <v>44139</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="33"/>
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>5</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -833,17 +857,18 @@
       <c r="C11" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="34"/>
+      <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>6.5</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>6.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -853,20 +878,18 @@
       <c r="C12" s="23">
         <v>44285</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="33"/>
+      <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="E12">
-        <v>1.5</v>
-      </c>
       <c r="F12">
+        <v>1.5</v>
+      </c>
+      <c r="G12">
         <v>1</v>
       </c>
-      <c r="G12">
-        <v>1.5</v>
-      </c>
       <c r="H12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -875,10 +898,13 @@
         <v>2</v>
       </c>
       <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -888,17 +914,18 @@
       <c r="C13" s="22">
         <v>44232</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="33"/>
+      <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>6</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -908,17 +935,18 @@
       <c r="C14" s="21">
         <v>44255</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="33"/>
+      <c r="E14" t="s">
         <v>25</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>6</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -928,94 +956,105 @@
       <c r="C15" s="20">
         <v>44285</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="33"/>
+      <c r="E15" t="s">
         <v>26</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>6</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="33"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B17" s="16">
         <v>44289</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C17" s="19">
         <v>44303</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" s="33"/>
+      <c r="E17" t="s">
         <v>21</v>
       </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <v>1.5</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>1.5</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-      <c r="K16">
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>1.5</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>1.5</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B18" s="17">
         <v>44304</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C18" s="18">
         <v>44317</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" s="33"/>
+      <c r="E18" t="s">
         <v>27</v>
       </c>
-      <c r="J17">
+      <c r="K18">
         <v>6</v>
       </c>
-      <c r="K17">
+      <c r="L18">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E18">
+      <c r="F19">
         <v>17.5</v>
       </c>
-      <c r="F18">
+      <c r="G19">
         <v>20</v>
       </c>
-      <c r="G18">
+      <c r="H19">
         <v>17</v>
       </c>
-      <c r="H18">
+      <c r="I19">
         <v>16.5</v>
       </c>
-      <c r="I18">
+      <c r="J19">
         <v>16.5</v>
       </c>
-      <c r="J18">
+      <c r="K19">
         <v>16</v>
       </c>
-      <c r="K18">
+      <c r="L19">
         <v>103.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed few fields in ScheduleApproximation.xlsx file
</commit_message>
<xml_diff>
--- a/ScheduleApproximation.xlsx
+++ b/ScheduleApproximation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s538339\Documents\GDP-1\health-wellness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F424F49-70D2-4E4F-A8B5-089B23888D3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1127228-B9DD-452B-ABE8-19A5EAAB3435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83925983-7E47-4241-A59F-1E401A86CA2F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <r>
       <t xml:space="preserve">                                                                                                                                                 </t>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Testing</t>
-  </si>
-  <si>
-    <t>Working Hours</t>
   </si>
 </sst>
 </file>
@@ -580,14 +577,15 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="44.90625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="4" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" customWidth="1"/>
     <col min="5" max="5" width="15.1796875" customWidth="1"/>
     <col min="6" max="6" width="11.08984375" customWidth="1"/>
     <col min="8" max="8" width="12.26953125" customWidth="1"/>
@@ -623,9 +621,7 @@
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
@@ -971,8 +967,12 @@
       <c r="A16" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
+      <c r="B16" s="25">
+        <v>44263</v>
+      </c>
+      <c r="C16" s="25">
+        <v>44287</v>
+      </c>
       <c r="D16" s="33"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated sprint 1 schedule
</commit_message>
<xml_diff>
--- a/ScheduleApproximation.xlsx
+++ b/ScheduleApproximation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s538339\Documents\GDP-1\health-wellness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2490D576-F728-48FC-A885-AEA436D46C81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F88B98B-5AF2-4732-BC1D-7225A47B0FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83925983-7E47-4241-A59F-1E401A86CA2F}"/>
   </bookViews>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629B0EE5-2389-44FF-B5B1-1268CBE07ED8}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,9 +654,7 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="6">
-        <v>31</v>
-      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
@@ -672,16 +670,16 @@
         <v>0</v>
       </c>
       <c r="E5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="6">
         <v>0</v>
       </c>
       <c r="G5" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="4">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -689,13 +687,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="6">
         <v>1</v>
@@ -704,10 +702,10 @@
         <v>2</v>
       </c>
       <c r="G6" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H6" s="4">
-        <v>9.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -721,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
@@ -730,10 +728,10 @@
         <v>2</v>
       </c>
       <c r="G7" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H7" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -744,22 +742,22 @@
         <v>2</v>
       </c>
       <c r="C8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="6">
         <v>1</v>
       </c>
       <c r="G8" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H8" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -767,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="6">
         <v>2</v>
@@ -782,10 +780,10 @@
         <v>2</v>
       </c>
       <c r="G9" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H9" s="4">
-        <v>10.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -797,11 +795,9 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6">
+      <c r="G10" s="6"/>
+      <c r="H10" s="4">
         <v>35</v>
-      </c>
-      <c r="H10" s="4">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated ScheduleApproximation.xlsx file by adding sprint 2
</commit_message>
<xml_diff>
--- a/ScheduleApproximation.xlsx
+++ b/ScheduleApproximation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s538339\Documents\GDP-1\health-wellness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F88B98B-5AF2-4732-BC1D-7225A47B0FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4B9110-5B95-4776-BE15-F2AA1B90B5E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83925983-7E47-4241-A59F-1E401A86CA2F}"/>
   </bookViews>
@@ -569,7 +569,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -667,19 +667,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="4">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -687,7 +687,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -705,7 +705,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -713,25 +713,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
       </c>
       <c r="F7" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" s="6">
         <v>2</v>
       </c>
       <c r="H7" s="4">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -739,10 +739,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -757,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -780,10 +780,10 @@
         <v>2</v>
       </c>
       <c r="G9" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H9" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -797,7 +797,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="4">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -805,13 +805,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="6">
         <v>3</v>
@@ -820,10 +820,10 @@
         <v>2</v>
       </c>
       <c r="G11" s="6">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="H11" s="4">
-        <v>6.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -831,7 +831,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
@@ -840,16 +840,16 @@
         <v>2</v>
       </c>
       <c r="E12" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G12" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H12" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -857,25 +857,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="6">
         <v>2</v>
       </c>
       <c r="G13" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H13" s="4">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -886,22 +886,22 @@
         <v>2</v>
       </c>
       <c r="C14" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14" s="6">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H14" s="4">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -913,11 +913,9 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="6">
-        <v>34</v>
-      </c>
+      <c r="G15" s="6"/>
       <c r="H15" s="4">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -928,19 +926,19 @@
         <v>2</v>
       </c>
       <c r="C16" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D16" s="6">
         <v>3</v>
       </c>
       <c r="E16" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G16" s="6">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -951,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
@@ -963,7 +961,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H17" s="4">
         <v>11</v>
@@ -980,16 +978,16 @@
         <v>2</v>
       </c>
       <c r="D18" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E18" s="6">
         <v>2</v>
       </c>
       <c r="F18" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G18" s="6">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H18" s="4">
         <v>6</v>
@@ -1006,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E19" s="6">
         <v>4</v>
@@ -1015,7 +1013,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H19" s="4">
         <v>103.5</v>

</xml_diff>

<commit_message>
Added sprint 3 data in ScheduleApproximation.xlsx file
</commit_message>
<xml_diff>
--- a/ScheduleApproximation.xlsx
+++ b/ScheduleApproximation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s538339\Documents\GDP-1\health-wellness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4B9110-5B95-4776-BE15-F2AA1B90B5E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528BF25F-B145-45BE-8A76-5E48FC6AE7CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83925983-7E47-4241-A59F-1E401A86CA2F}"/>
   </bookViews>
@@ -185,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -228,11 +228,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -252,6 +263,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629B0EE5-2389-44FF-B5B1-1268CBE07ED8}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -940,6 +953,9 @@
       <c r="G16" s="6">
         <v>1</v>
       </c>
+      <c r="H16" s="11">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
@@ -964,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="4">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -990,7 +1006,7 @@
         <v>4</v>
       </c>
       <c r="H18" s="4">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1016,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="4">
-        <v>103.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1028,8 +1044,9 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="6">
-        <v>30</v>
+      <c r="G20" s="6"/>
+      <c r="H20" s="12">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Sprint 4 data updated
</commit_message>
<xml_diff>
--- a/ScheduleApproximation.xlsx
+++ b/ScheduleApproximation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s538339\Documents\GDP-1\health-wellness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528BF25F-B145-45BE-8A76-5E48FC6AE7CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF3851C-32F3-4114-A8CF-93AEF4A7630A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83925983-7E47-4241-A59F-1E401A86CA2F}"/>
   </bookViews>
@@ -185,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -239,11 +239,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -265,6 +274,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629B0EE5-2389-44FF-B5B1-1268CBE07ED8}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,10 +809,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
+    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -814,78 +822,63 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6">
-        <v>2</v>
-      </c>
-      <c r="C11" s="6">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6">
-        <v>2</v>
-      </c>
-      <c r="E11" s="6">
-        <v>3</v>
-      </c>
-      <c r="F11" s="6">
-        <v>2</v>
-      </c>
-      <c r="G11" s="6">
-        <v>4</v>
-      </c>
-      <c r="H11" s="4">
-        <v>16</v>
-      </c>
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6">
+        <v>3</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3</v>
+      </c>
+      <c r="F12" s="6">
+        <v>2</v>
+      </c>
+      <c r="G12" s="6">
         <v>4</v>
       </c>
-      <c r="C12" s="6">
-        <v>2</v>
-      </c>
-      <c r="D12" s="6">
-        <v>2</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6">
-        <v>4</v>
-      </c>
-      <c r="G12" s="6">
-        <v>2</v>
-      </c>
       <c r="H12" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
         <v>4</v>
       </c>
-      <c r="E13" s="6">
-        <v>2</v>
-      </c>
-      <c r="F13" s="6">
-        <v>2</v>
-      </c>
       <c r="G13" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13" s="4">
         <v>15</v>
@@ -893,274 +886,336 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+      <c r="G14" s="6">
+        <v>3</v>
+      </c>
+      <c r="H14" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
-        <v>2</v>
-      </c>
-      <c r="C14" s="6">
+      <c r="B15" s="6">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
         <v>4</v>
       </c>
-      <c r="D14" s="6">
-        <v>3</v>
-      </c>
-      <c r="E14" s="6">
-        <v>2</v>
-      </c>
-      <c r="F14" s="6">
-        <v>3</v>
-      </c>
-      <c r="G14" s="6">
-        <v>2</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="D15" s="6">
+        <v>3</v>
+      </c>
+      <c r="E15" s="6">
+        <v>2</v>
+      </c>
+      <c r="F15" s="6">
+        <v>3</v>
+      </c>
+      <c r="G15" s="6">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="4">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6">
-        <v>2</v>
-      </c>
-      <c r="C16" s="6">
-        <v>4</v>
-      </c>
-      <c r="D16" s="6">
-        <v>3</v>
-      </c>
-      <c r="E16" s="6">
-        <v>3</v>
-      </c>
-      <c r="F16" s="6">
-        <v>3</v>
-      </c>
-      <c r="G16" s="6">
-        <v>1</v>
-      </c>
-      <c r="H16" s="11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6">
-        <v>3</v>
-      </c>
-      <c r="F17" s="6">
-        <v>2</v>
-      </c>
-      <c r="G17" s="6">
-        <v>2</v>
-      </c>
-      <c r="H17" s="4">
-        <v>18</v>
-      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="6">
         <v>3</v>
       </c>
       <c r="G18" s="6">
-        <v>4</v>
-      </c>
-      <c r="H18" s="4">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="H18" s="11">
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6">
+        <v>3</v>
+      </c>
+      <c r="F19" s="6">
+        <v>2</v>
+      </c>
+      <c r="G19" s="6">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
-        <v>1</v>
-      </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6">
-        <v>2</v>
-      </c>
-      <c r="E19" s="6">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="6">
+        <v>3</v>
+      </c>
+      <c r="C20" s="6">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6">
         <v>4</v>
       </c>
-      <c r="F19" s="6">
-        <v>1</v>
-      </c>
-      <c r="G19" s="6">
-        <v>2</v>
-      </c>
-      <c r="H19" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="12">
-        <v>63</v>
+      <c r="E20" s="6">
+        <v>2</v>
+      </c>
+      <c r="F20" s="6">
+        <v>3</v>
+      </c>
+      <c r="G20" s="6">
+        <v>4</v>
+      </c>
+      <c r="H20" s="4">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="6">
         <v>2</v>
       </c>
       <c r="E21" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F21" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6">
-        <v>2</v>
-      </c>
-      <c r="C22" s="6">
-        <v>2</v>
-      </c>
-      <c r="D22" s="6">
-        <v>1</v>
-      </c>
-      <c r="E22" s="6">
-        <v>3</v>
-      </c>
-      <c r="F22" s="6">
-        <v>1</v>
-      </c>
-      <c r="G22" s="6">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="H21" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="12">
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="6">
-        <v>2</v>
-      </c>
-      <c r="D23" s="6">
-        <v>2</v>
-      </c>
-      <c r="E23" s="6">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6">
-        <v>2</v>
-      </c>
-      <c r="G23" s="6">
-        <v>7</v>
-      </c>
+      <c r="A23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="6">
+        <v>4</v>
+      </c>
+      <c r="C24" s="6">
+        <v>3</v>
+      </c>
+      <c r="D24" s="6">
+        <v>2</v>
+      </c>
+      <c r="E24" s="6">
+        <v>2</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6">
+        <v>2</v>
+      </c>
+      <c r="H24" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="6">
+        <v>2</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6">
+        <v>3</v>
+      </c>
+      <c r="F25" s="6">
+        <v>2</v>
+      </c>
+      <c r="G25" s="6">
+        <v>3</v>
+      </c>
+      <c r="H25" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6">
+        <v>2</v>
+      </c>
+      <c r="D26" s="6">
+        <v>2</v>
+      </c>
+      <c r="E26" s="6">
+        <v>3</v>
+      </c>
+      <c r="F26" s="6">
+        <v>2</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1</v>
+      </c>
+      <c r="H26" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
-        <v>0</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-      <c r="D24" s="6">
-        <v>3</v>
-      </c>
-      <c r="E24" s="6">
-        <v>2</v>
-      </c>
-      <c r="F24" s="6">
-        <v>3</v>
-      </c>
-      <c r="G24" s="6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="B27" s="6">
+        <v>2</v>
+      </c>
+      <c r="C27" s="6">
+        <v>2</v>
+      </c>
+      <c r="D27" s="6">
+        <v>3</v>
+      </c>
+      <c r="E27" s="6">
+        <v>2</v>
+      </c>
+      <c r="F27" s="6">
+        <v>3</v>
+      </c>
+      <c r="G27" s="6">
+        <v>2</v>
+      </c>
+      <c r="H27" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H28" s="13">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B29" s="5">
         <v>23</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C29" s="5">
         <v>18</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D29" s="5">
         <v>31</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E29" s="5">
         <v>33</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F29" s="5">
         <v>25</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G29" s="5">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final changes made to ScheduleApproximation.xlsx file
</commit_message>
<xml_diff>
--- a/ScheduleApproximation.xlsx
+++ b/ScheduleApproximation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s538339\Documents\GDP-1\health-wellness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF3851C-32F3-4114-A8CF-93AEF4A7630A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B784B0AA-5012-4CAA-9120-4016E4FBB95F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{83925983-7E47-4241-A59F-1E401A86CA2F}"/>
   </bookViews>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629B0EE5-2389-44FF-B5B1-1268CBE07ED8}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,7 +716,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="6">
         <v>1</v>
@@ -728,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -800,13 +800,13 @@
         <v>1</v>
       </c>
       <c r="F9" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="6">
         <v>3</v>
       </c>
       <c r="H9" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -818,7 +818,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="4">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -843,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="6">
         <v>3</v>
@@ -852,10 +852,10 @@
         <v>2</v>
       </c>
       <c r="G12" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H12" s="4">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -875,13 +875,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" s="6">
         <v>2</v>
       </c>
       <c r="H13" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -945,7 +945,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="4">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -973,7 +973,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="6">
         <v>3</v>
@@ -982,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="11">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1022,7 +1022,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="6">
         <v>2</v>
@@ -1031,10 +1031,10 @@
         <v>3</v>
       </c>
       <c r="G20" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H20" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1051,7 +1051,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" s="6">
         <v>1</v>
@@ -1060,7 +1060,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1072,7 +1072,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="12">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1153,7 +1153,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" s="6">
         <v>2</v>
@@ -1162,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="11">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1193,7 +1193,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H28" s="13">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1201,22 +1201,25 @@
         <v>24</v>
       </c>
       <c r="B29" s="5">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C29" s="5">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D29" s="5">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E29" s="5">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F29" s="5">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G29" s="5">
-        <v>130</v>
+        <v>35</v>
+      </c>
+      <c r="H29" s="13">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>